<commit_message>
[Documentation] Weekly Report - 9
</commit_message>
<xml_diff>
--- a/Documentation/Project Weekly Report - FHF - 9.xlsx
+++ b/Documentation/Project Weekly Report - FHF - 9.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F608B5-4C65-456E-967E-22BF3D28FA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60196746-F2C0-45A5-A5D3-D21B41C68934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wx" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
   <si>
     <t>PROJECT REPORT</t>
   </si>
@@ -197,15 +197,9 @@
     <t>HuyenBN</t>
   </si>
   <si>
-    <t>Not finished</t>
-  </si>
-  <si>
     <t>AnNT</t>
   </si>
   <si>
-    <t>Study Angular</t>
-  </si>
-  <si>
     <t>Study OCE LOT</t>
   </si>
   <si>
@@ -218,18 +212,9 @@
     <t>Code: Login with Google</t>
   </si>
   <si>
-    <t>GiangNT, HuyenBN</t>
-  </si>
-  <si>
     <t>ThongPQ</t>
   </si>
   <si>
-    <t>Continue Coding main functionalities</t>
-  </si>
-  <si>
-    <t>Continue Updating documentations</t>
-  </si>
-  <si>
     <t>KienNT</t>
   </si>
   <si>
@@ -239,21 +224,9 @@
     <t>Landlord Upload House Information</t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
-    <t>Styling in progress</t>
-  </si>
-  <si>
-    <t>Waiting for registration with Google</t>
-  </si>
-  <si>
     <t>GiangNT</t>
   </si>
   <si>
-    <t>Study OData</t>
-  </si>
-  <si>
     <t>Design Front-end for Pages</t>
   </si>
   <si>
@@ -263,9 +236,6 @@
     <t>KienNT, HuyenBN</t>
   </si>
   <si>
-    <t>Database Population</t>
-  </si>
-  <si>
     <t>(Landlord) Manage Rooms</t>
   </si>
   <si>
@@ -281,7 +251,49 @@
     <t>Home Page: Search &amp; Filter with OData</t>
   </si>
   <si>
-    <t>24/10/2022-30/10/2022</t>
+    <t>31/10/2022-06/11/2022</t>
+  </si>
+  <si>
+    <t>Design Front-end + Angular + API</t>
+  </si>
+  <si>
+    <t>(Guest) House Detail, Room Detail</t>
+  </si>
+  <si>
+    <t>Database Design &amp; Population</t>
+  </si>
+  <si>
+    <t>Finished with testing accounts</t>
+  </si>
+  <si>
+    <t>Home Page</t>
+  </si>
+  <si>
+    <t>Finish coding, Update style</t>
+  </si>
+  <si>
+    <t>(Landlord) Upload House Information</t>
+  </si>
+  <si>
+    <t>2 methods</t>
+  </si>
+  <si>
+    <t>Fix bugs</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>Documentation: Report 4</t>
+  </si>
+  <si>
+    <t>Submission</t>
+  </si>
+  <si>
+    <t>Test Web Responsive directly on Mobile Phone</t>
+  </si>
+  <si>
+    <t>By running localhost on internal wifi</t>
   </si>
 </sst>
 </file>
@@ -745,26 +757,26 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="3" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="41.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="57.42578125" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="4"/>
+    <col min="1" max="1" width="6.44140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="57.44140625" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="8.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -772,20 +784,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -802,142 +814,144 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>26</v>
@@ -946,40 +960,29 @@
         <v>7</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>4</v>
       </c>
@@ -996,43 +999,33 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>1</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>4</v>
       </c>
@@ -1049,99 +1042,133 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D26" s="9">
         <v>44723</v>
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="D27" s="9">
         <v>44723</v>
       </c>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D28" s="9">
         <v>44723</v>
       </c>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>4</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="9">
+        <v>44723</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>5</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="9">
+        <v>44723</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>6</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="9">
+        <v>44723</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="9"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="9"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="9"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>4</v>
       </c>
@@ -1158,35 +1185,45 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>1</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="9">
+        <v>44815</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>

</xml_diff>

<commit_message>
[Documentation] Weekly Report - 10
</commit_message>
<xml_diff>
--- a/Documentation/Project Weekly Report - FHF - 9.xlsx
+++ b/Documentation/Project Weekly Report - FHF - 9.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60196746-F2C0-45A5-A5D3-D21B41C68934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782AB883-7EFE-476B-B856-196CB50C171E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wx" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
   <si>
     <t>PROJECT REPORT</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>By running localhost on internal wifi</t>
+  </si>
+  <si>
+    <t>13/11/2022</t>
   </si>
 </sst>
 </file>
@@ -757,26 +760,26 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="41.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="57.44140625" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="8.6640625" style="4"/>
+    <col min="1" max="1" width="6.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="57.42578125" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -784,7 +787,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -792,12 +795,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -814,7 +817,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -831,7 +834,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -846,7 +849,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -863,7 +866,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -878,7 +881,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -895,7 +898,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>6</v>
       </c>
@@ -912,7 +915,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -929,7 +932,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -946,7 +949,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>9</v>
       </c>
@@ -963,26 +966,26 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>4</v>
       </c>
@@ -999,33 +1002,33 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>4</v>
       </c>
@@ -1042,7 +1045,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -1052,12 +1055,12 @@
       <c r="C26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="9">
-        <v>44723</v>
+      <c r="D26" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2</v>
       </c>
@@ -1067,14 +1070,14 @@
       <c r="C27" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="9">
-        <v>44723</v>
+      <c r="D27" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>3</v>
       </c>
@@ -1084,14 +1087,14 @@
       <c r="C28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="9">
-        <v>44723</v>
+      <c r="D28" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>4</v>
       </c>
@@ -1101,14 +1104,14 @@
       <c r="C29" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="9">
-        <v>44723</v>
+      <c r="D29" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>5</v>
       </c>
@@ -1118,14 +1121,14 @@
       <c r="C30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="9">
-        <v>44723</v>
+      <c r="D30" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>6</v>
       </c>
@@ -1135,40 +1138,40 @@
       <c r="C31" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="9">
-        <v>44723</v>
+      <c r="D31" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="9"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="9"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="9"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>4</v>
       </c>
@@ -1185,7 +1188,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>1</v>
       </c>
@@ -1202,28 +1205,28 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>

</xml_diff>